<commit_message>
Merapikan maximo-columns.sql Menambahkan excel TBC untuk verifikasi terkair custom column
</commit_message>
<xml_diff>
--- a/Integration Services Project/mapping/TBC Custom Column.xlsx
+++ b/Integration Services Project/mapping/TBC Custom Column.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\STE.2022.CoswinMigration_2\Integration Services Project\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1484D45C-10FD-447E-8351-200CBCBCC91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEBDFCA-5A7A-454D-B57B-E8CFCD8B1270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{30AE3FD5-A676-41AA-BE3F-A8C11DC10E47}"/>
   </bookViews>
@@ -104,12 +104,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{D23CDD40-BA3F-401B-B102-B529000992C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di mapping</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{300B82B5-C562-49D4-BED9-23E0690E5149}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+belum ada di mapping, tapi ada di script</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>objectname</t>
   </si>
@@ -130,13 +178,37 @@
   </si>
   <si>
     <t>ste_cswndonum</t>
+  </si>
+  <si>
+    <t>ASSETMETER</t>
+  </si>
+  <si>
+    <t>STE_CSWNCONSTANT</t>
+  </si>
+  <si>
+    <t>STE_CSWNFORECAST</t>
+  </si>
+  <si>
+    <t>STE_CSWNFREQUENCY</t>
+  </si>
+  <si>
+    <t>STE_CSWNFREQUENCYUNIT</t>
+  </si>
+  <si>
+    <t>STE_CSWNSTARTDATE</t>
+  </si>
+  <si>
+    <t>STE_CSWNTOTALCUMRUNUNIT</t>
+  </si>
+  <si>
+    <t>ste_mtlastread</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +228,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -494,16 +579,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD5A254-79FD-4D7A-99EB-9D3569F45B3B}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -538,6 +623,62 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
update note in TBC file
</commit_message>
<xml_diff>
--- a/Integration Services Project/mapping/TBC Custom Column.xlsx
+++ b/Integration Services Project/mapping/TBC Custom Column.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\STE.2022.CoswinMigration_2\Integration Services Project\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD908FAB-5248-4452-B6C1-418F3375182B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA12D9C-A56E-43CA-A088-AC67A3321B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{30AE3FD5-A676-41AA-BE3F-A8C11DC10E47}"/>
   </bookViews>
@@ -124,7 +124,127 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Belum ada di mapping</t>
+Belum ada di mapping, tapi sudah ada di script</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{8C4E5750-AFE0-49E8-818D-5A11324CE8EA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di mapping, tapi sudah ada di script</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{BC1EFB49-6000-4020-9163-810DE2A927A2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di mapping, tapi sudah ada di script</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{89356591-26DA-46FE-A1A4-7E0277C74B25}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di mapping, tapi sudah ada di script</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{7BF43B16-0D67-40CD-AF09-70A88539959F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di mapping, tapi sudah ada di script</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{D51A0400-DAA3-475A-8EBD-33B589A75E48}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di mapping, tapi sudah ada di script</t>
         </r>
       </text>
     </comment>
@@ -173,6 +293,126 @@
           </rPr>
           <t xml:space="preserve">
 Belum ada di Mapping</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{DC51E7C5-BBC6-4A0B-A0DA-6F4DE6B4CCD9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di Mapping</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{77B4928B-9D44-4F5E-80FC-93CDE4A9AA6D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di mapping tapi ada di script</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{505456DC-60F1-4E87-8810-B72F26612832}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di mapping, tapi ada di script</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{C88C28C1-1C7C-49E8-9C69-C91EC0DA2567}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di mapping, tapi ada di script</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{2E435809-14E5-4B81-B6F6-7C92D09C0583}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Belum ada di mapping, tapi ada di script</t>
         </r>
       </text>
     </comment>
@@ -181,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>objectname</t>
   </si>
@@ -235,6 +475,27 @@
   </si>
   <si>
     <t>STE_MIGRATIONNSITEMPK</t>
+  </si>
+  <si>
+    <t>ste_cswnrecwo</t>
+  </si>
+  <si>
+    <t>matrectrans</t>
+  </si>
+  <si>
+    <t>Line 665 dan 666 di sheet 0003 purchase order sepertinya salah kode package dan nama table, harusnya matrectrans bukan matusetrans</t>
+  </si>
+  <si>
+    <t>ste_cswnctrycd</t>
+  </si>
+  <si>
+    <t>ste_cswnctryname</t>
+  </si>
+  <si>
+    <t>ste_cswndpt</t>
+  </si>
+  <si>
+    <t>CURRENCY</t>
   </si>
 </sst>
 </file>
@@ -621,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD5A254-79FD-4D7A-99EB-9D3569F45B3B}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,6 +998,43 @@
         <v>17</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>